<commit_message>
pridanie tracklistu Drum and Bass 2024 Mix #4
</commit_message>
<xml_diff>
--- a/concatenate-TemplateString-Tracks.xlsx
+++ b/concatenate-TemplateString-Tracks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="264">
   <si>
     <t> `&lt;div class='track'&gt;</t>
   </si>
@@ -576,102 +576,6 @@
     <t xml:space="preserve"> Chimera</t>
   </si>
   <si>
-    <t xml:space="preserve">0:00:00 Nu:Tone </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> One Day At A Time (ft. Lalin St. Juste)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:03:41 Rezilient </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Positive Reaction </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:07:21 Keeno &amp; Thomas Oliver </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sunflowers </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:10:40 Thomas Oliver </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Friendly Fire (Danny Byrd Remix) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:13:59 Nu:Logic </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Day &amp; Night </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:17:17 Break feat. Kyo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gave Too Much </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:20:36 Break </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hope (feat. Celestine) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:23:10 Prestige </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> One Big Place </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:26:07 Camo &amp; Krooked </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Turn Up (The Music) (Pola &amp; Bryson Remix) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:29:26 Revaux </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Colours (ft. Charli Brix) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:34:57 Kumarion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Instinct </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:36:48 Enei &amp; Kasra </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Projections (Mefjus Remix) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:39:22 Document One &amp; Levela </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Steppa</t>
-  </si>
-  <si>
-    <t>Styke</t>
-  </si>
-  <si>
-    <t>Stride</t>
-  </si>
-  <si>
-    <t>Hugh Hardie</t>
-  </si>
-  <si>
-    <t>Darjeeling</t>
-  </si>
-  <si>
-    <t>Ruckspin, Ruth Royal</t>
-  </si>
-  <si>
-    <t>Porcelain</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -723,88 +627,187 @@
     <t>017</t>
   </si>
   <si>
-    <t>Full Circle (DJ Marky Remix)</t>
-  </si>
-  <si>
-    <t>Charli Brix, Visages</t>
-  </si>
-  <si>
-    <t>Terror, Espa</t>
-  </si>
-  <si>
-    <t>Loaded Gun</t>
-  </si>
-  <si>
-    <t>Styke, Auris</t>
-  </si>
-  <si>
-    <t>Mellifluous</t>
-  </si>
-  <si>
-    <t>Shibumi</t>
-  </si>
-  <si>
-    <t>Sings</t>
-  </si>
-  <si>
-    <t>Askel, Becca Jane Grey</t>
-  </si>
-  <si>
-    <t>Goodbye VIP</t>
-  </si>
-  <si>
-    <t>Document One</t>
-  </si>
-  <si>
-    <t>Like This</t>
-  </si>
-  <si>
-    <t>DLR, Hoppa</t>
-  </si>
-  <si>
-    <t>A World That Looked The Same</t>
-  </si>
-  <si>
-    <t>Alibi, Nitri</t>
-  </si>
-  <si>
-    <t>No Escape</t>
-  </si>
-  <si>
-    <t>Keeno, Telomic</t>
-  </si>
-  <si>
-    <t>Listen Close</t>
-  </si>
-  <si>
-    <t>Sustance, Charli Brix</t>
-  </si>
-  <si>
-    <t>Break the Habit</t>
-  </si>
-  <si>
-    <t>Revaux</t>
-  </si>
-  <si>
-    <t>Ibex</t>
-  </si>
-  <si>
-    <t>DOT, Kyrist</t>
-  </si>
-  <si>
-    <t>Arbus (Kyrist Remix)</t>
-  </si>
-  <si>
-    <t>Never Lost (Ill Truth Remix)</t>
-  </si>
-  <si>
-    <t>Constrict</t>
-  </si>
-  <si>
-    <t>Visages, Messy MC</t>
-  </si>
-  <si>
-    <t>Para Days</t>
+    <t>001 Andromedik, Lexurus, Nu-La - Adrenaline</t>
+  </si>
+  <si>
+    <t>002 Culture Shock - Get To Me</t>
+  </si>
+  <si>
+    <t>003 Delta Heavy, Cameron Warren - Bad Decisions</t>
+  </si>
+  <si>
+    <t>004 Friction, Metrik - Ultrafunk</t>
+  </si>
+  <si>
+    <t>005 Sub Focus, Gene Farris - It's Time</t>
+  </si>
+  <si>
+    <t>006 Tantrum Desire - Rhythm</t>
+  </si>
+  <si>
+    <t>007 Break - All You Gotta Do</t>
+  </si>
+  <si>
+    <t>008 Crystal Clear - Wavey</t>
+  </si>
+  <si>
+    <t>009 Fourward - Countdown (Instrumental Mix)</t>
+  </si>
+  <si>
+    <t>010 Kalane - Frost</t>
+  </si>
+  <si>
+    <t>011 Waeys - This Tune</t>
+  </si>
+  <si>
+    <t>012 Trail, Monty - Wraith</t>
+  </si>
+  <si>
+    <t>013 Trail, Visages - Comet</t>
+  </si>
+  <si>
+    <t>014 DJ Marky, XRS, Makoto - Soul Samba (DJ Marky &amp; Makoto Remix 2024)</t>
+  </si>
+  <si>
+    <t>015 Shy FX, Mr. Williamz, KingH - Gideon's Charge (feat. KINGH)</t>
+  </si>
+  <si>
+    <t>016 SOLAH - Stick Around</t>
+  </si>
+  <si>
+    <t>017 DJ Marky, Pola &amp; Bryson, IYAMAH - Be There</t>
+  </si>
+  <si>
+    <t>018 Blue Marble - Time to Love Again</t>
+  </si>
+  <si>
+    <t>019 Dope Ammo, Taiwan Mc, Ed Solo - Babylon Falling (Ed Solo Remix)</t>
+  </si>
+  <si>
+    <t>020 Ruth Royall - Feels Like Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adrenaline</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Get To Me</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delta Heavy, Cameron Warren </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bad Decisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Friction, Metrik </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ultrafunk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sub Focus, Gene Farris </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It's Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rhythm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Break </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All You Gotta Do</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Crystal Clear </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wavey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fourward </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Countdown (Instrumental Mix)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kalane </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Frost</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Waeys </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This Tune</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trail, Monty </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wraith</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trail, Visages </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJ Marky, XRS, Makoto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soul Samba (DJ Marky &amp; Makoto Remix 2024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shy FX, Mr. Williamz, KingH </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gideon's Charge (feat. KINGH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SOLAH </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stick Around</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DJ Marky, Pola &amp; Bryson, IYAMAH </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Be There</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Blue Marble </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time to Love Again</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dope Ammo, Taiwan Mc, Ed Solo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Babylon Falling (Ed Solo Remix)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ruth Royall </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feels Like Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Andromedik, Lexurus, Nu-La</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14:O30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14:O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1374,13 +1377,13 @@
     </row>
     <row r="14" spans="1:36" ht="15.75" thickTop="1">
       <c r="A14" s="8" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>24</v>
@@ -1393,39 +1396,39 @@
       </c>
       <c r="O14" s="3" t="str">
         <f>CONCATENATE($I$13,$I$14,A14,$I$16,$I$17,$I$18,$I$19,$I$20,B14,I$22,$I$23,$I$24,$I$25,$I$26,C14,$I$28,$I$29)</f>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;001&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Styke&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Stride&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;001&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Andromedik, Lexurus, Nu-La&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Adrenaline&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ14" s="4"/>
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="8" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>214</v>
+        <v>149</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="13" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="3" t="str">
-        <f t="shared" ref="O15:O30" si="0">CONCATENATE($I$13,$I$14,A15,$I$16,$I$17,$I$18,$I$19,$I$20,B15,I$22,$I$23,$I$24,$I$25,$I$26,C15,$I$28,$I$29)</f>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;002&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Hugh Hardie&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Darjeeling&lt;/div&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="O15:O33" si="0">CONCATENATE($I$13,$I$14,A15,$I$16,$I$17,$I$18,$I$19,$I$20,B15,I$22,$I$23,$I$24,$I$25,$I$26,C15,$I$28,$I$29)</f>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;002&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Culture Shock &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Get To Me&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ15" s="4"/>
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="8" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>24</v>
@@ -1435,19 +1438,19 @@
       </c>
       <c r="O16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;003&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Ruckspin, Ruth Royal&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Porcelain&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;003&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Delta Heavy, Cameron Warren &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Bad Decisions&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ16" s="4"/>
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="8" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>24</v>
@@ -1457,19 +1460,19 @@
       </c>
       <c r="O17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;004&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Charli Brix, Visages&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Full Circle (DJ Marky Remix)&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;004&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Friction, Metrik &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Ultrafunk&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ17" s="4"/>
     </row>
     <row r="18" spans="1:36">
       <c r="A18" s="8" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>24</v>
@@ -1479,19 +1482,19 @@
       </c>
       <c r="O18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;005&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Terror, Espa&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Loaded Gun&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;005&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Sub Focus, Gene Farris &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; It's Time&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ18" s="4"/>
     </row>
     <row r="19" spans="1:36">
       <c r="A19" s="8" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>239</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>24</v>
@@ -1501,19 +1504,19 @@
       </c>
       <c r="O19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;006&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Styke, Auris&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Mellifluous&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;006&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Tantrum Desire &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Rhythm&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ19" s="4"/>
     </row>
     <row r="20" spans="1:36">
       <c r="A20" s="8" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>25</v>
@@ -1523,19 +1526,19 @@
       </c>
       <c r="O20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;007&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Shibumi&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Sings&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;007&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Break &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; All You Gotta Do&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ20" s="4"/>
     </row>
     <row r="21" spans="1:36">
       <c r="A21" s="8" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="13" t="s">
@@ -1543,19 +1546,19 @@
       </c>
       <c r="O21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;008&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Askel, Becca Jane Grey&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Goodbye VIP&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;008&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Crystal Clear &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Wavey&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ21" s="4"/>
     </row>
     <row r="22" spans="1:36">
       <c r="A22" s="8" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>24</v>
@@ -1565,19 +1568,19 @@
       </c>
       <c r="O22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;009&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Document One&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Like This&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;009&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Fourward &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Countdown (Instrumental Mix)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ22" s="4"/>
     </row>
     <row r="23" spans="1:36">
       <c r="A23" s="8" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>24</v>
@@ -1587,19 +1590,19 @@
       </c>
       <c r="O23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;010&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;DLR, Hoppa&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;A World That Looked The Same&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;010&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Kalane &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Frost&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ23" s="4"/>
     </row>
     <row r="24" spans="1:36">
       <c r="A24" s="8" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>24</v>
@@ -1609,19 +1612,19 @@
       </c>
       <c r="O24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;011&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Alibi, Nitri&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;No Escape&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;011&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Waeys &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; This Tune&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ24" s="4"/>
     </row>
     <row r="25" spans="1:36">
       <c r="A25" s="8" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>24</v>
@@ -1631,19 +1634,19 @@
       </c>
       <c r="O25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;012&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Keeno, Telomic&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Listen Close&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;012&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Trail, Monty &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Wraith&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ25" s="4"/>
     </row>
     <row r="26" spans="1:36">
       <c r="A26" s="8" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>24</v>
@@ -1653,19 +1656,19 @@
       </c>
       <c r="O26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;013&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Sustance, Charli Brix&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Break the Habit&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;013&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Trail, Visages &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Comet&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ26" s="4"/>
     </row>
     <row r="27" spans="1:36">
       <c r="A27" s="8" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="13" t="s">
@@ -1673,19 +1676,19 @@
       </c>
       <c r="O27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;014&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Revaux&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Ibex&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;014&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; DJ Marky, XRS, Makoto &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Soul Samba (DJ Marky &amp; Makoto Remix 2024)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ27" s="4"/>
     </row>
     <row r="28" spans="1:36">
       <c r="A28" s="8" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>24</v>
@@ -1695,19 +1698,19 @@
       </c>
       <c r="O28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;015&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;DOT, Kyrist&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Arbus (Kyrist Remix)&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;015&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Shy FX, Mr. Williamz, KingH &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Gideon's Charge (feat. KINGH)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ28" s="4"/>
     </row>
     <row r="29" spans="1:36" ht="15.75" thickBot="1">
       <c r="A29" s="8" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>24</v>
@@ -1717,42 +1720,72 @@
       </c>
       <c r="O29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;016&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Constrict&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Never Lost (Ill Truth Remix)&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;016&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; SOLAH &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Stick Around&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ29" s="4"/>
     </row>
     <row r="30" spans="1:36">
       <c r="A30" s="8" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="O30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;017&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; DJ Marky, Pola &amp; Bryson, IYAMAH &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Be There&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="AJ30" s="4"/>
+    </row>
+    <row r="31" spans="1:36">
+      <c r="A31" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="B31" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="O31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;018&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Blue Marble &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Time to Love Again&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="AJ31" s="4"/>
+    </row>
+    <row r="32" spans="1:36">
+      <c r="A32" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="O30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;017&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Visages, Messy MC&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Para Days&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="AJ30" s="4"/>
-    </row>
-    <row r="31" spans="1:36">
-      <c r="A31" s="8"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="AJ31" s="4"/>
-    </row>
-    <row r="32" spans="1:36">
-      <c r="A32" s="8"/>
-      <c r="B32" s="1"/>
-      <c r="C32"/>
+      <c r="B32" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C32" t="s">
+        <v>257</v>
+      </c>
+      <c r="O32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;019&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Dope Ammo, Taiwan Mc, Ed Solo &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Babylon Falling (Ed Solo Remix)&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
       <c r="AJ32" s="4"/>
     </row>
     <row r="33" spans="1:36">
-      <c r="A33" s="8"/>
-      <c r="B33" s="1"/>
-      <c r="C33"/>
+      <c r="A33" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" t="s">
+        <v>259</v>
+      </c>
+      <c r="O33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;020&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Ruth Royall &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Feels Like Home&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
       <c r="AJ33" s="4"/>
     </row>
     <row r="34" spans="1:36">
@@ -1987,8 +2020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:F46"/>
+    <sheetView topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="G53" sqref="F34:G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1999,7 +2032,7 @@
     <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="62" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="62" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -2695,310 +2728,446 @@
       <c r="B32"/>
       <c r="F32"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:7">
       <c r="A33"/>
       <c r="B33"/>
       <c r="F33"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>186</v>
-      </c>
-      <c r="B34" t="s">
-        <v>187</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="B34"/>
       <c r="C34" s="1" t="str">
-        <f>MID(A34,1,7)</f>
-        <v>0:00:00</v>
+        <f>MID(A34,1,3)</f>
+        <v>001</v>
       </c>
       <c r="E34" s="1" t="str">
-        <f>MID(A34,8,100)</f>
-        <v xml:space="preserve"> Nu:Tone </v>
+        <f>MID(A34,4,100)</f>
+        <v xml:space="preserve"> Andromedik, Lexurus, Nu-La - Adrenaline</v>
       </c>
       <c r="F34" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>260</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>188</v>
-      </c>
-      <c r="B35" t="s">
-        <v>189</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="B35"/>
       <c r="C35" s="1" t="str">
-        <f t="shared" ref="C35:C46" si="3">MID(A35,1,7)</f>
-        <v>0:03:41</v>
+        <f t="shared" ref="C35:C56" si="3">MID(A35,1,3)</f>
+        <v>002</v>
       </c>
       <c r="E35" s="1" t="str">
-        <f t="shared" ref="E35:E46" si="4">MID(A35,8,100)</f>
-        <v xml:space="preserve"> Rezilient </v>
+        <f t="shared" ref="E35:E55" si="4">MID(A35,4,100)</f>
+        <v xml:space="preserve"> Culture Shock - Get To Me</v>
       </c>
       <c r="F35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>149</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>190</v>
-      </c>
-      <c r="B36" t="s">
-        <v>191</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B36"/>
       <c r="C36" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:07:21</v>
+        <v>003</v>
       </c>
       <c r="E36" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Keeno &amp; Thomas Oliver </v>
+        <v xml:space="preserve"> Delta Heavy, Cameron Warren - Bad Decisions</v>
       </c>
       <c r="F36" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>225</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>192</v>
-      </c>
-      <c r="B37" t="s">
-        <v>193</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="B37"/>
       <c r="C37" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:10:40</v>
+        <v>004</v>
       </c>
       <c r="E37" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Thomas Oliver </v>
+        <v xml:space="preserve"> Friction, Metrik - Ultrafunk</v>
       </c>
       <c r="F37" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>227</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>194</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:13:59</v>
+        <v>005</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Nu:Logic </v>
+        <v xml:space="preserve"> Sub Focus, Gene Farris - It's Time</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>229</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>196</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:17:17</v>
+        <v>006</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Break feat. Kyo </v>
+        <v xml:space="preserve"> Tantrum Desire - Rhythm</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>32</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:20:36</v>
+        <v>007</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Break </v>
+        <v xml:space="preserve"> Break - All You Gotta Do</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>232</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>200</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:23:10</v>
+        <v>008</v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Prestige </v>
+        <v xml:space="preserve"> Crystal Clear - Wavey</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>234</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>202</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:26:07</v>
+        <v>009</v>
       </c>
       <c r="E42" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Camo &amp; Krooked </v>
+        <v xml:space="preserve"> Fourward - Countdown (Instrumental Mix)</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>236</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>204</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:29:26</v>
+        <v>010</v>
       </c>
       <c r="E43" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Revaux </v>
+        <v xml:space="preserve"> Kalane - Frost</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>238</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:34:57</v>
+        <v>011</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Kumarion </v>
+        <v xml:space="preserve"> Waeys - This Tune</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>240</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>208</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:36:48</v>
+        <v>012</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Enei &amp; Kasra </v>
+        <v xml:space="preserve"> Trail, Monty - Wraith</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>242</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>210</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>0:39:22</v>
+        <v>013</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> Document One &amp; Levela </v>
+        <v xml:space="preserve"> Trail, Visages - Comet</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50"/>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51"/>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52"/>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53"/>
-    </row>
-    <row r="54" spans="1:1">
+        <v>244</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>216</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>014</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> DJ Marky, XRS, Makoto - Soul Samba (DJ Marky &amp; Makoto Remix 2024)</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>217</v>
+      </c>
+      <c r="C48" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>015</v>
+      </c>
+      <c r="E48" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> Shy FX, Mr. Williamz, KingH - Gideon's Charge (feat. KINGH)</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>218</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>016</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> SOLAH - Stick Around</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>219</v>
+      </c>
+      <c r="C50" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>017</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> DJ Marky, Pola &amp; Bryson, IYAMAH - Be There</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>018</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> Blue Marble - Time to Love Again</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>221</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>019</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> Dope Ammo, Taiwan Mc, Ed Solo - Babylon Falling (Ed Solo Remix)</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>222</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>020</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> Ruth Royall - Feels Like Home</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54"/>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="C54" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E54" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55"/>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="C55" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E55" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56"/>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="C56" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:7">
       <c r="A58"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:7">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:7">
       <c r="A60"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:7">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:7">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:7">
       <c r="A63" s="6"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:7">
       <c r="A64" s="6"/>
     </row>
     <row r="65" spans="1:1">

</xml_diff>

<commit_message>
pridanie tracklistu #5 MIX 2024
</commit_message>
<xml_diff>
--- a/concatenate-TemplateString-Tracks.xlsx
+++ b/concatenate-TemplateString-Tracks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="255">
   <si>
     <t> `&lt;div class='track'&gt;</t>
   </si>
@@ -117,18 +117,6 @@
     <t xml:space="preserve"> Tantrum Desire </t>
   </si>
   <si>
-    <t xml:space="preserve"> Document One </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dossa &amp; Locuzzed </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amoss </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dephzac </t>
-  </si>
-  <si>
     <t xml:space="preserve">001 AKOV </t>
   </si>
   <si>
@@ -354,228 +342,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>00:00:00 - - - - Pola &amp; Bryson, Lauren Archer - Under</t>
-  </si>
-  <si>
-    <t>00:04:13 - - - - Manikin - Reflection</t>
-  </si>
-  <si>
-    <t>00:08:38 - - - - Levela, A Little Sound - Moving Forward</t>
-  </si>
-  <si>
-    <t>00:10:50 - - - - Monrroe, Zara Kershaw - Out of Time</t>
-  </si>
-  <si>
-    <t>00:13:42 - - - - Dephzac - Jazzpark - Original Mix</t>
-  </si>
-  <si>
-    <t>00:16:16 - - - - Netsky, Digital Farm Animals - Rio (feat. Digital Farm Animals)</t>
-  </si>
-  <si>
-    <t>00:19:12 - - - - Culture Shock - Lost</t>
-  </si>
-  <si>
-    <t>00:22:09 - - - - Mat Zo - Vice</t>
-  </si>
-  <si>
-    <t>00:24:21 - - - - Dossa &amp; Locuzzed - Brainfunk</t>
-  </si>
-  <si>
-    <t>00:27:40 - - - - Tantrum Desire - Resistance</t>
-  </si>
-  <si>
-    <t>00:31:00 - - - - Annix, A Little Sound - Overload</t>
-  </si>
-  <si>
-    <t>00:33:33 - - - - Kasra, Enei, DRS - Overthinking</t>
-  </si>
-  <si>
-    <t>00:36:52 - - - - Kumarion - Lilith</t>
-  </si>
-  <si>
-    <t>00:39:48 - - - - Insomniax, InsideInfo - Facehugger - Insideinfo Remix</t>
-  </si>
-  <si>
-    <t>00:43:07 - - - - Subtension - Left Handed</t>
-  </si>
-  <si>
-    <t>00:46:26 - - - - Quadrant, Iris - Cold Brew</t>
-  </si>
-  <si>
-    <t>00:50:28 - - - - Document One - Follow Me</t>
-  </si>
-  <si>
-    <t>00:53:25 - - - - Murdock, Dynamite MC, Enei - Dark Cloud - Enei Remix</t>
-  </si>
-  <si>
-    <t>00:57:06 - - - - Document One, Levela - Dials</t>
-  </si>
-  <si>
-    <t>01:00:24 - - - - Mefjus, Calyx &amp; TeeBee - Fractured - Calyx &amp; TeeBee Remix</t>
-  </si>
-  <si>
-    <t>01:03:21 - - - - Kyrist – Chimera</t>
-  </si>
-  <si>
-    <t>01:07:01 - - - - Tantrum Desire - Nationwide Rocker</t>
-  </si>
-  <si>
-    <t>01:10:20 - - - - Mr Traumatik, Terrence &amp; Phillip - Skin Suit - Terrence &amp; Phillip Flip</t>
-  </si>
-  <si>
-    <t>01:14:01 - - - - Amoss - Tinnies &amp; Ciggies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01:17:41 - - - - Phibes - Got to see her VIP - VIP  </t>
-  </si>
-  <si>
-    <t>01:20:49 - - - - Phibes - Why Should I </t>
-  </si>
-  <si>
-    <t>01:24:07 - - - - Bou, Mefjus – Wormhole</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pola &amp; Bryson, Lauren Archer </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Under</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Manikin </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reflection</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Levela, A Little Sound </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Moving Forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Monrroe, Zara Kershaw </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Out of Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Netsky, Digital Farm Animals </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rio (feat. Digital Farm Animals)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Culture Shock </t>
   </si>
   <si>
-    <t xml:space="preserve"> Lost</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mat Zo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vice</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Brainfunk</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Resistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Annix, A Little Sound </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Overload</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kasra, Enei, DRS </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Overthinking</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kumarion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lilith</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Insomniax, InsideInfo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Subtension </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Left Handed</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quadrant, Iris </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cold Brew</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Follow Me</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Murdock, Dynamite MC, Enei </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Document One, Levela </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dials</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mefjus, Calyx &amp; TeeBee </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nationwide Rocker</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mr Traumatik, Terrence &amp; Phillip </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tinnies &amp; Ciggies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Phibes </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Why Should I </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kyrist  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jazzpark  (Original Mix)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Facehugger  (Insideinfo Remix)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dark Cloud  (Enei Remix)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fractured (Calyx &amp; TeeBee Remix)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Skin Suit (Terrence &amp; Phillip Flip)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Got to see her (VIP ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bou, Mefjus  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wormhole</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chimera</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -808,6 +577,210 @@
   </si>
   <si>
     <t>020</t>
+  </si>
+  <si>
+    <t>001 Keeno - Branches</t>
+  </si>
+  <si>
+    <t>002 Dimension, Alison Wonderland - Satellite (SOTA Remix)</t>
+  </si>
+  <si>
+    <t>003 Chicane, Bryan Adams - Don't Give Up (Grafix Remix)</t>
+  </si>
+  <si>
+    <t>004 Aktive - Loko</t>
+  </si>
+  <si>
+    <t>005 Maduk, Lexurus, Crooked Bangs - Follow My Heart</t>
+  </si>
+  <si>
+    <t>006 Waeys - Stopping Turning</t>
+  </si>
+  <si>
+    <t>007 Fred V, Dnmo, Paul Dowling - Collide</t>
+  </si>
+  <si>
+    <t>008 Freddy B, Emperor - Swarm</t>
+  </si>
+  <si>
+    <t>009 Wilkinson, Emily Makis - Break It Down (feat. Emily Makis)</t>
+  </si>
+  <si>
+    <t>010 Sub Focus - Wildfire</t>
+  </si>
+  <si>
+    <t>011 Chris Lorenzo - Pump (1991 Remix)</t>
+  </si>
+  <si>
+    <t>012 Makoto, L-Side - Settle Down</t>
+  </si>
+  <si>
+    <t>013 Andromedik, Rani - Bleed The Same</t>
+  </si>
+  <si>
+    <t>014 Total Science, S.P.Y- - Gangsta (Watch the Ride Remix)</t>
+  </si>
+  <si>
+    <t>015 Blue Marble - Je Me Souviendrai</t>
+  </si>
+  <si>
+    <t>016 Level 2 - Bite the Bone</t>
+  </si>
+  <si>
+    <t>017 Funkstar De Luxe, Fred V - Sun Is Shining</t>
+  </si>
+  <si>
+    <t>018 Enei - Want It</t>
+  </si>
+  <si>
+    <t>018 Friction, ÆON-MODE, Blanke, Lauren L’aimant - State Of Mind</t>
+  </si>
+  <si>
+    <t>019 DLR - Brain Eaters</t>
+  </si>
+  <si>
+    <t>020 Delta Heavy, You - Babylon</t>
+  </si>
+  <si>
+    <t>021 DJ Marky, SOLAH - Poetry</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>Aktive - Loko</t>
+  </si>
+  <si>
+    <t>Keeno</t>
+  </si>
+  <si>
+    <t>Dimension, Alison Wonderland</t>
+  </si>
+  <si>
+    <t>Chicane, Bryan Adams</t>
+  </si>
+  <si>
+    <t>Maduk, Lexurus, Crooked Bangs</t>
+  </si>
+  <si>
+    <t>Waeys</t>
+  </si>
+  <si>
+    <t>Fred V, Dnmo, Paul Dowling</t>
+  </si>
+  <si>
+    <t>Freddy B, Emperor</t>
+  </si>
+  <si>
+    <t>Wilkinson, Emily Makis</t>
+  </si>
+  <si>
+    <t>Sub Focus</t>
+  </si>
+  <si>
+    <t>Chris Lorenzo</t>
+  </si>
+  <si>
+    <t>Makoto, L-Side</t>
+  </si>
+  <si>
+    <t>Andromedik, Rani</t>
+  </si>
+  <si>
+    <t>Total Science, S.P.Y</t>
+  </si>
+  <si>
+    <t>Blue Marble</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Funkstar De Luxe, Fred V</t>
+  </si>
+  <si>
+    <t>Enei</t>
+  </si>
+  <si>
+    <t>Friction, ÆON-MODE, Blanke, Lauren L’aimant</t>
+  </si>
+  <si>
+    <t>DLR</t>
+  </si>
+  <si>
+    <t>Delta Heavy, You</t>
+  </si>
+  <si>
+    <t>DJ Marky, SOLAH</t>
+  </si>
+  <si>
+    <t>Poetry</t>
+  </si>
+  <si>
+    <t>Babylon</t>
+  </si>
+  <si>
+    <t>Brain Eaters</t>
+  </si>
+  <si>
+    <t>State Of Mind</t>
+  </si>
+  <si>
+    <t>Want It</t>
+  </si>
+  <si>
+    <t>Sun Is Shining</t>
+  </si>
+  <si>
+    <t>Bite the Bone</t>
+  </si>
+  <si>
+    <t>Je Me Souviendrai</t>
+  </si>
+  <si>
+    <t>Gangsta (Watch the Ride Remix)</t>
+  </si>
+  <si>
+    <t>Bleed The Same</t>
+  </si>
+  <si>
+    <t>Settle Down</t>
+  </si>
+  <si>
+    <t>Pump (1991 Remix)</t>
+  </si>
+  <si>
+    <t>Wildfire</t>
+  </si>
+  <si>
+    <t>Break It Down (feat. Emily Makis)</t>
+  </si>
+  <si>
+    <t>Swarm</t>
+  </si>
+  <si>
+    <t>Collide</t>
+  </si>
+  <si>
+    <t>Stopping Turning</t>
+  </si>
+  <si>
+    <t>Follow My Heart</t>
+  </si>
+  <si>
+    <t>Loko</t>
+  </si>
+  <si>
+    <t>Don't Give Up (Grafix Remix)</t>
+  </si>
+  <si>
+    <t>Satellite (SOTA Remix)</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>022</t>
   </si>
 </sst>
 </file>
@@ -946,7 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -958,7 +931,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1265,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14:O33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14:O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1279,7 +1251,7 @@
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="14" width="9.140625" style="3"/>
-    <col min="15" max="15" width="29.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="221.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -1335,13 +1307,13 @@
     </row>
     <row r="10" spans="1:36" ht="15.75" thickBot="1"/>
     <row r="11" spans="1:36">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1355,8 +1327,8 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:36" ht="15.75" thickBot="1">
       <c r="A13" s="5" t="s">
@@ -1368,27 +1340,28 @@
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="15.75" thickTop="1">
       <c r="A14" s="8" t="s">
-        <v>186</v>
+        <v>109</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C14" t="s">
-        <v>223</v>
-      </c>
-      <c r="H14" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14"/>
+      <c r="H14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="12" t="s">
         <v>28</v>
       </c>
       <c r="N14" s="3" t="s">
@@ -1396,407 +1369,448 @@
       </c>
       <c r="O14" s="3" t="str">
         <f>CONCATENATE($I$13,$I$14,A14,$I$16,$I$17,$I$18,$I$19,$I$20,B14,I$22,$I$23,$I$24,$I$25,$I$26,C14,$I$28,$I$29)</f>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;001&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Andromedik, Lexurus, Nu-La&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Adrenaline&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;001&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Keeno&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Branches&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ14" s="4"/>
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="8" t="s">
-        <v>187</v>
+        <v>110</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="3" t="str">
-        <f t="shared" ref="O15:O33" si="0">CONCATENATE($I$13,$I$14,A15,$I$16,$I$17,$I$18,$I$19,$I$20,B15,I$22,$I$23,$I$24,$I$25,$I$26,C15,$I$28,$I$29)</f>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;002&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Culture Shock &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Get To Me&lt;/div&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="O15:O36" si="0">CONCATENATE($I$13,$I$14,A15,$I$16,$I$17,$I$18,$I$19,$I$20,B15,I$22,$I$23,$I$24,$I$25,$I$26,C15,$I$28,$I$29)</f>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;002&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Dimension, Alison Wonderland&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Satellite (SOTA Remix)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ15" s="4"/>
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="8" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="H16" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16"/>
+      <c r="H16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>23</v>
       </c>
       <c r="O16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;003&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Delta Heavy, Cameron Warren &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Bad Decisions&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;003&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Chicane, Bryan Adams&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Don't Give Up (Grafix Remix)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ16" s="4"/>
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H17" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D17"/>
+      <c r="H17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="12" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;004&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Friction, Metrik &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Ultrafunk&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;004&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Aktive - Loko&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Loko&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ17" s="4"/>
     </row>
     <row r="18" spans="1:36">
       <c r="A18" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="H18" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18"/>
+      <c r="H18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="12" t="s">
         <v>8</v>
       </c>
       <c r="O18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;005&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Sub Focus, Gene Farris &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; It's Time&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;005&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Maduk, Lexurus, Crooked Bangs&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Follow My Heart&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ18" s="4"/>
     </row>
     <row r="19" spans="1:36">
       <c r="A19" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="H19" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19"/>
+      <c r="H19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="12" t="s">
         <v>23</v>
       </c>
       <c r="O19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;006&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Tantrum Desire &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Rhythm&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;006&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Waeys&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Stopping Turning&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ19" s="4"/>
     </row>
     <row r="20" spans="1:36">
       <c r="A20" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="H20" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20"/>
+      <c r="H20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>30</v>
       </c>
       <c r="O20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;007&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Break &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; All You Gotta Do&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;007&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Fred V, Dnmo, Paul Dowling&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Collide&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ20" s="4"/>
     </row>
     <row r="21" spans="1:36">
       <c r="A21" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12" t="s">
         <v>26</v>
       </c>
       <c r="O21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;008&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Crystal Clear &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Wavey&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;008&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Freddy B, Emperor&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Swarm&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ21" s="4"/>
     </row>
     <row r="22" spans="1:36">
       <c r="A22" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="H22" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D22"/>
+      <c r="H22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="12" t="s">
         <v>23</v>
       </c>
       <c r="O22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;009&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Fourward &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Countdown (Instrumental Mix)&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;009&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Wilkinson, Emily Makis&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Break It Down (feat. Emily Makis)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ22" s="4"/>
     </row>
     <row r="23" spans="1:36">
       <c r="A23" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H23" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D23"/>
+      <c r="H23" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="12" t="s">
         <v>31</v>
       </c>
       <c r="O23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;010&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Kalane &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Frost&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;010&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Sub Focus&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Wildfire&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ23" s="4"/>
     </row>
     <row r="24" spans="1:36">
       <c r="A24" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="H24" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24"/>
+      <c r="H24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="12" t="s">
         <v>11</v>
       </c>
       <c r="O24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;011&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Waeys &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; This Tune&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;011&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Chris Lorenzo&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Pump (1991 Remix)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ24" s="4"/>
     </row>
     <row r="25" spans="1:36">
       <c r="A25" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H25" s="12" t="s">
+      <c r="D25"/>
+      <c r="H25" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="12" t="s">
         <v>23</v>
       </c>
       <c r="O25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;012&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Trail, Monty &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Wraith&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;012&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Makoto, L-Side&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Settle Down&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ25" s="4"/>
     </row>
     <row r="26" spans="1:36">
       <c r="A26" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="H26" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26"/>
+      <c r="H26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="12" t="s">
         <v>27</v>
       </c>
       <c r="O26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;013&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Trail, Visages &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Comet&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;013&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Andromedik, Rani&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Bleed The Same&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ26" s="4"/>
     </row>
     <row r="27" spans="1:36">
       <c r="A27" s="8" t="s">
-        <v>199</v>
+        <v>122</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D27"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12" t="s">
         <v>10</v>
       </c>
       <c r="O27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;014&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; DJ Marky, XRS, Makoto &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Soul Samba (DJ Marky &amp; Makoto Remix 2024)&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;014&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Total Science, S.P.Y&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Gangsta (Watch the Ride Remix)&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ27" s="4"/>
     </row>
     <row r="28" spans="1:36">
       <c r="A28" s="8" t="s">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="H28" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D28"/>
+      <c r="H28" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="12" t="s">
         <v>23</v>
       </c>
       <c r="O28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;015&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Shy FX, Mr. Williamz, KingH &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Gideon's Charge (feat. KINGH)&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;015&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Blue Marble&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Je Me Souviendrai&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ28" s="4"/>
     </row>
     <row r="29" spans="1:36" ht="15.75" thickBot="1">
       <c r="A29" s="8" t="s">
-        <v>201</v>
+        <v>124</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H29" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D29"/>
+      <c r="H29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="I29" s="14" t="s">
         <v>23</v>
       </c>
       <c r="O29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;016&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; SOLAH &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Stick Around&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;016&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Level 2&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Bite the Bone&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ29" s="4"/>
     </row>
     <row r="30" spans="1:36">
       <c r="A30" s="8" t="s">
-        <v>202</v>
+        <v>125</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>253</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D30"/>
       <c r="O30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;017&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; DJ Marky, Pola &amp; Bryson, IYAMAH &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Be There&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;017&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Funkstar De Luxe, Fred V&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Sun Is Shining&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ30" s="4"/>
     </row>
     <row r="31" spans="1:36">
       <c r="A31" s="8" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>255</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="D31"/>
       <c r="O31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;018&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Blue Marble &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Time to Love Again&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;018&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Friction, ÆON-MODE, Blanke, Lauren L’aimant&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;State Of Mind&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ31" s="4"/>
     </row>
     <row r="32" spans="1:36">
       <c r="A32" s="8" t="s">
-        <v>262</v>
+        <v>185</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C32" t="s">
-        <v>257</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D32"/>
       <c r="O32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;019&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Dope Ammo, Taiwan Mc, Ed Solo &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Babylon Falling (Ed Solo Remix)&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;019&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Enei&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Want It&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ32" s="4"/>
     </row>
     <row r="33" spans="1:36">
       <c r="A33" s="8" t="s">
-        <v>263</v>
+        <v>186</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C33" t="s">
-        <v>259</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D33"/>
       <c r="O33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;020&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt; Ruth Royall &lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt; Feels Like Home&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;020&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;DLR&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Brain Eaters&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="AJ33" s="4"/>
     </row>
     <row r="34" spans="1:36">
-      <c r="A34" s="8"/>
-      <c r="B34" s="1"/>
-      <c r="C34"/>
+      <c r="A34" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D34"/>
+      <c r="O34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;021&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;Delta Heavy, You&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Babylon&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
     </row>
     <row r="35" spans="1:36">
-      <c r="A35" s="8"/>
-      <c r="B35" s="1"/>
-      <c r="C35"/>
+      <c r="A35" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D35"/>
+      <c r="O35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='track'&gt;&lt;div class='trackNumber'&gt;022&lt;/div&gt;&lt;div class='trackSeparator'&gt;|&lt;/div&gt;&lt;div class='trackArtist'&gt;DJ Marky, SOLAH&lt;/div&gt;&lt;div class='trackDash'&gt;-&lt;/div&gt;&lt;div class='trackName'&gt;Poetry&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
     </row>
     <row r="36" spans="1:36">
       <c r="A36" s="8"/>
@@ -2020,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="G53" sqref="F34:G53"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I22" sqref="H1:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2040,675 +2054,411 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A1"/>
       <c r="B1"/>
-      <c r="C1" s="1" t="str">
-        <f>MID(A1,2,8)</f>
-        <v xml:space="preserve">0:00:00 </v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <f>MID(A1,2,100)</f>
-        <v>0:00:00 - - - - Pola &amp; Bryson, Lauren Archer - Under</v>
+      <c r="E1" t="s">
+        <v>187</v>
       </c>
       <c r="F1" s="1" t="str">
-        <f>MID(E1,16,100)</f>
-        <v xml:space="preserve"> Pola &amp; Bryson, Lauren Archer - Under</v>
+        <f>MID(E1,5,100)</f>
+        <v>Keeno - Branches</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>140</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
+      <c r="A2"/>
       <c r="B2"/>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C29" si="0">MID(A2,2,8)</f>
-        <v xml:space="preserve">0:04:13 </v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E27" si="1">MID(A2,2,100)</f>
-        <v>0:04:13 - - - - Manikin - Reflection</v>
+      <c r="E2" t="s">
+        <v>188</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f t="shared" ref="F2:F27" si="2">MID(E2,16,100)</f>
-        <v xml:space="preserve"> Manikin - Reflection</v>
+        <f>MID(E2,5,100)</f>
+        <v>Dimension, Alison Wonderland - Satellite (SOTA Remix)</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>141</v>
+        <v>212</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>114</v>
-      </c>
+      <c r="A3"/>
       <c r="B3"/>
-      <c r="C3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:08:38 </v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:08:38 - - - - Levela, A Little Sound - Moving Forward</v>
+      <c r="E3" t="s">
+        <v>189</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Levela, A Little Sound - Moving Forward</v>
+        <f>MID(E3,5,100)</f>
+        <v>Chicane, Bryan Adams - Don't Give Up (Grafix Remix)</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>143</v>
+        <v>213</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>144</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:10:50 </v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:10:50 - - - - Monrroe, Zara Kershaw - Out of Time</v>
+      <c r="A4"/>
+      <c r="E4" t="s">
+        <v>190</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Monrroe, Zara Kershaw - Out of Time</v>
+        <f>MID(E4,5,100)</f>
+        <v>Aktive - Loko</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>146</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
+      <c r="A5"/>
       <c r="B5"/>
-      <c r="C5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:13:42 </v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:13:42 - - - - Dephzac - Jazzpark - Original Mix</v>
+      <c r="E5" t="s">
+        <v>191</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Dephzac - Jazzpark - Original Mix</v>
+        <f>MID(E5,5,100)</f>
+        <v>Maduk, Lexurus, Crooked Bangs - Follow My Heart</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>36</v>
+        <v>214</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>177</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>117</v>
-      </c>
+      <c r="A6"/>
       <c r="B6"/>
-      <c r="C6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:16:16 </v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:16:16 - - - - Netsky, Digital Farm Animals - Rio (feat. Digital Farm Animals)</v>
+      <c r="E6" t="s">
+        <v>192</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Netsky, Digital Farm Animals - Rio (feat. Digital Farm Animals)</v>
+        <f>MID(E6,5,100)</f>
+        <v>Waeys - Stopping Turning</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>147</v>
+        <v>215</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>148</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>118</v>
-      </c>
+      <c r="A7"/>
       <c r="B7"/>
-      <c r="C7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:19:12 </v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:19:12 - - - - Culture Shock - Lost</v>
+      <c r="E7" t="s">
+        <v>193</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Culture Shock - Lost</v>
+        <f>MID(E7,5,100)</f>
+        <v>Fred V, Dnmo, Paul Dowling - Collide</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>150</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>119</v>
-      </c>
+      <c r="A8"/>
       <c r="B8"/>
-      <c r="C8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:22:09 </v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:22:09 - - - - Mat Zo - Vice</v>
+      <c r="E8" t="s">
+        <v>194</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Mat Zo - Vice</v>
+        <f>MID(E8,5,100)</f>
+        <v>Freddy B, Emperor - Swarm</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>120</v>
-      </c>
+      <c r="A9"/>
       <c r="B9"/>
-      <c r="C9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:24:21 </v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:24:21 - - - - Dossa &amp; Locuzzed - Brainfunk</v>
+      <c r="E9" t="s">
+        <v>195</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Dossa &amp; Locuzzed - Brainfunk</v>
+        <f>MID(E9,5,100)</f>
+        <v>Wilkinson, Emily Makis - Break It Down (feat. Emily Makis)</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>218</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>153</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>121</v>
-      </c>
+      <c r="A10"/>
       <c r="B10"/>
-      <c r="C10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:27:40 </v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:27:40 - - - - Tantrum Desire - Resistance</v>
+      <c r="E10" t="s">
+        <v>196</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Tantrum Desire - Resistance</v>
+        <f>MID(E10,5,100)</f>
+        <v>Sub Focus - Wildfire</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
+        <v>219</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>122</v>
-      </c>
+      <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:31:00 </v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:31:00 - - - - Annix, A Little Sound - Overload</v>
+      <c r="E11" t="s">
+        <v>197</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Annix, A Little Sound - Overload</v>
+        <f>MID(E11,5,100)</f>
+        <v>Chris Lorenzo - Pump (1991 Remix)</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>155</v>
+        <v>220</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>156</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>123</v>
-      </c>
+      <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:33:33 </v>
-      </c>
-      <c r="E12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:33:33 - - - - Kasra, Enei, DRS - Overthinking</v>
+      <c r="E12" t="s">
+        <v>198</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Kasra, Enei, DRS - Overthinking</v>
+        <f>MID(E12,5,100)</f>
+        <v>Makoto, L-Side - Settle Down</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>157</v>
+        <v>221</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>124</v>
-      </c>
+      <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:36:52 </v>
-      </c>
-      <c r="E13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:36:52 - - - - Kumarion - Lilith</v>
+      <c r="E13" t="s">
+        <v>199</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Kumarion - Lilith</v>
+        <f>MID(E13,5,100)</f>
+        <v>Andromedik, Rani - Bleed The Same</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>160</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>125</v>
-      </c>
+      <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:39:48 </v>
-      </c>
-      <c r="E14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:39:48 - - - - Insomniax, InsideInfo - Facehugger - Insideinfo Remix</v>
+      <c r="E14" t="s">
+        <v>200</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Insomniax, InsideInfo - Facehugger - Insideinfo Remix</v>
+        <f>MID(E14,5,100)</f>
+        <v>Total Science, S.P.Y- - Gangsta (Watch the Ride Remix)</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>161</v>
+        <v>223</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>178</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>126</v>
-      </c>
+      <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:43:07 </v>
-      </c>
-      <c r="E15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:43:07 - - - - Subtension - Left Handed</v>
+      <c r="E15" t="s">
+        <v>201</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Subtension - Left Handed</v>
+        <f>MID(E15,5,100)</f>
+        <v>Blue Marble - Je Me Souviendrai</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>163</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>127</v>
-      </c>
+      <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:46:26 </v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:46:26 - - - - Quadrant, Iris - Cold Brew</v>
+      <c r="E16" t="s">
+        <v>202</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Quadrant, Iris - Cold Brew</v>
+        <f>MID(E16,5,100)</f>
+        <v>Level 2 - Bite the Bone</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>164</v>
+        <v>225</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>128</v>
-      </c>
+      <c r="A17"/>
       <c r="B17"/>
-      <c r="C17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:50:28 </v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:50:28 - - - - Document One - Follow Me</v>
+      <c r="E17" t="s">
+        <v>203</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Document One - Follow Me</v>
+        <f>MID(E17,5,100)</f>
+        <v>Funkstar De Luxe, Fred V - Sun Is Shining</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>33</v>
+        <v>226</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>166</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>129</v>
-      </c>
+      <c r="A18"/>
       <c r="B18"/>
-      <c r="C18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:53:25 </v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:53:25 - - - - Murdock, Dynamite MC, Enei - Dark Cloud - Enei Remix</v>
+      <c r="E18" t="s">
+        <v>204</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Murdock, Dynamite MC, Enei - Dark Cloud - Enei Remix</v>
+        <f>MID(E18,5,100)</f>
+        <v>Enei - Want It</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>167</v>
+        <v>228</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>179</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>130</v>
-      </c>
+      <c r="A19"/>
       <c r="B19"/>
-      <c r="C19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">0:57:06 </v>
-      </c>
-      <c r="E19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>0:57:06 - - - - Document One, Levela - Dials</v>
+      <c r="E19" t="s">
+        <v>205</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Document One, Levela - Dials</v>
+        <f>MID(E19,5,100)</f>
+        <v>Friction, ÆON-MODE, Blanke, Lauren L’aimant - State Of Mind</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>168</v>
+        <v>227</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>131</v>
-      </c>
+      <c r="A20"/>
       <c r="B20"/>
-      <c r="C20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:00:24 </v>
-      </c>
-      <c r="E20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>1:00:24 - - - - Mefjus, Calyx &amp; TeeBee - Fractured - Calyx &amp; TeeBee Remix</v>
+      <c r="E20" t="s">
+        <v>206</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Mefjus, Calyx &amp; TeeBee - Fractured - Calyx &amp; TeeBee Remix</v>
+        <f>MID(E20,5,100)</f>
+        <v>DLR - Brain Eaters</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>180</v>
+        <v>234</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" t="s">
-        <v>132</v>
-      </c>
+      <c r="A21"/>
       <c r="B21"/>
-      <c r="C21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:03:21 </v>
-      </c>
-      <c r="E21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>1:03:21 - - - - Kyrist – Chimera</v>
+      <c r="E21" t="s">
+        <v>207</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Kyrist – Chimera</v>
+        <f>MID(E21,5,100)</f>
+        <v>Delta Heavy, You - Babylon</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>176</v>
+        <v>230</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>133</v>
-      </c>
+      <c r="A22"/>
       <c r="B22"/>
-      <c r="C22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:07:01 </v>
-      </c>
-      <c r="E22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>1:07:01 - - - - Tantrum Desire - Nationwide Rocker</v>
+      <c r="E22" t="s">
+        <v>208</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Tantrum Desire - Nationwide Rocker</v>
+        <f>MID(E22,5,100)</f>
+        <v>DJ Marky, SOLAH - Poetry</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>171</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>134</v>
-      </c>
+      <c r="A23"/>
       <c r="B23"/>
-      <c r="C23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:10:20 </v>
-      </c>
-      <c r="E23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>1:10:20 - - - - Mr Traumatik, Terrence &amp; Phillip - Skin Suit - Terrence &amp; Phillip Flip</v>
-      </c>
-      <c r="F23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Mr Traumatik, Terrence &amp; Phillip - Skin Suit - Terrence &amp; Phillip Flip</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" t="s">
-        <v>135</v>
-      </c>
+      <c r="A24"/>
       <c r="B24"/>
-      <c r="C24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:14:01 </v>
-      </c>
-      <c r="E24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>1:14:01 - - - - Amoss - Tinnies &amp; Ciggies</v>
-      </c>
-      <c r="F24" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Amoss - Tinnies &amp; Ciggies</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" t="s">
-        <v>136</v>
-      </c>
+      <c r="A25"/>
       <c r="B25"/>
-      <c r="C25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:17:41 </v>
-      </c>
-      <c r="E25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">1:17:41 - - - - Phibes - Got to see her VIP - VIP  </v>
-      </c>
-      <c r="F25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Phibes - Got to see her VIP - VIP  </v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>137</v>
-      </c>
+      <c r="A26"/>
       <c r="B26"/>
-      <c r="C26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:20:49 </v>
-      </c>
-      <c r="E26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>1:20:49 - - - - Phibes - Why Should I </v>
-      </c>
-      <c r="F26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Phibes - Why Should I </v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>138</v>
-      </c>
+      <c r="A27"/>
       <c r="B27"/>
-      <c r="C27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">1:24:07 </v>
-      </c>
-      <c r="E27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>1:24:07 - - - - Bou, Mefjus – Wormhole</v>
-      </c>
-      <c r="F27" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> Bou, Mefjus – Wormhole</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28"/>
       <c r="B28"/>
-      <c r="C28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="F28"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C2:C29" si="0">MID(A29,2,8)</f>
         <v/>
       </c>
       <c r="F29"/>
@@ -2735,7 +2485,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>203</v>
+        <v>126</v>
       </c>
       <c r="B34"/>
       <c r="C34" s="1" t="str">
@@ -2747,402 +2497,402 @@
         <v xml:space="preserve"> Andromedik, Lexurus, Nu-La - Adrenaline</v>
       </c>
       <c r="F34" t="s">
-        <v>260</v>
+        <v>183</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>223</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>204</v>
+        <v>127</v>
       </c>
       <c r="B35"/>
       <c r="C35" s="1" t="str">
-        <f t="shared" ref="C35:C56" si="3">MID(A35,1,3)</f>
+        <f t="shared" ref="C35:C56" si="1">MID(A35,1,3)</f>
         <v>002</v>
       </c>
       <c r="E35" s="1" t="str">
-        <f t="shared" ref="E35:E55" si="4">MID(A35,4,100)</f>
+        <f t="shared" ref="E35:E55" si="2">MID(A35,4,100)</f>
         <v xml:space="preserve"> Culture Shock - Get To Me</v>
       </c>
       <c r="F35" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>224</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>205</v>
+        <v>128</v>
       </c>
       <c r="B36"/>
       <c r="C36" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>003</v>
       </c>
       <c r="E36" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Delta Heavy, Cameron Warren - Bad Decisions</v>
       </c>
       <c r="F36" t="s">
-        <v>225</v>
+        <v>148</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>226</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>206</v>
+        <v>129</v>
       </c>
       <c r="B37"/>
       <c r="C37" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>004</v>
       </c>
       <c r="E37" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Friction, Metrik - Ultrafunk</v>
       </c>
       <c r="F37" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>228</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>207</v>
+        <v>130</v>
       </c>
       <c r="C38" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>005</v>
       </c>
       <c r="E38" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Sub Focus, Gene Farris - It's Time</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>229</v>
+        <v>152</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>230</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>208</v>
+        <v>131</v>
       </c>
       <c r="C39" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>006</v>
       </c>
       <c r="E39" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Tantrum Desire - Rhythm</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>231</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>209</v>
+        <v>132</v>
       </c>
       <c r="C40" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>007</v>
       </c>
       <c r="E40" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Break - All You Gotta Do</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>232</v>
+        <v>155</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>233</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>210</v>
+        <v>133</v>
       </c>
       <c r="C41" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>008</v>
       </c>
       <c r="E41" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Crystal Clear - Wavey</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>235</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="C42" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>009</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Fourward - Countdown (Instrumental Mix)</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>236</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>237</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>212</v>
+        <v>135</v>
       </c>
       <c r="C43" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>010</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Kalane - Frost</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>238</v>
+        <v>161</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>239</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>011</v>
       </c>
       <c r="E44" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Waeys - This Tune</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>240</v>
+        <v>163</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>241</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
       <c r="C45" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>012</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Trail, Monty - Wraith</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>242</v>
+        <v>165</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>243</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>215</v>
+        <v>138</v>
       </c>
       <c r="C46" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>013</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Trail, Visages - Comet</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>244</v>
+        <v>167</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>245</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>216</v>
+        <v>139</v>
       </c>
       <c r="C47" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>014</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> DJ Marky, XRS, Makoto - Soul Samba (DJ Marky &amp; Makoto Remix 2024)</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>246</v>
+        <v>169</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>247</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>217</v>
+        <v>140</v>
       </c>
       <c r="C48" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>015</v>
       </c>
       <c r="E48" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Shy FX, Mr. Williamz, KingH - Gideon's Charge (feat. KINGH)</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>248</v>
+        <v>171</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>218</v>
+        <v>141</v>
       </c>
       <c r="C49" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>016</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> SOLAH - Stick Around</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>250</v>
+        <v>173</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>251</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>142</v>
       </c>
       <c r="C50" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>017</v>
       </c>
       <c r="E50" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> DJ Marky, Pola &amp; Bryson, IYAMAH - Be There</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>252</v>
+        <v>175</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>253</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>220</v>
+        <v>143</v>
       </c>
       <c r="C51" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>018</v>
       </c>
       <c r="E51" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Blue Marble - Time to Love Again</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>254</v>
+        <v>177</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>255</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>221</v>
+        <v>144</v>
       </c>
       <c r="C52" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>019</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Dope Ammo, Taiwan Mc, Ed Solo - Babylon Falling (Ed Solo Remix)</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>256</v>
+        <v>179</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>257</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>222</v>
+        <v>145</v>
       </c>
       <c r="C53" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>020</v>
       </c>
       <c r="E53" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve"> Ruth Royall - Feels Like Home</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>258</v>
+        <v>181</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>259</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54"/>
       <c r="C54" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E54" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55"/>
       <c r="C55" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="E55" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56"/>
       <c r="C56" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3184,7 +2934,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="A1:B37"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3196,298 +2946,298 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>